<commit_message>
Updated r_v and h_p parameters with mean values for test 15mmol_20C
</commit_message>
<xml_diff>
--- a/Separator Model/Input/15mmolNa2CO3_20C.xlsx
+++ b/Separator Model/Input/15mmolNa2CO3_20C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Projekte\MA-Model_3\Separator Model\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagr9\Projekte\MA\MA-Model_3\Separator Model\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E42A3EC-6460-4C7F-8C61-3E7992F949CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C17E8E-F16F-401E-9240-119948B408ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{E05DA534-964F-48A7-BAA6-64E8E844F20B}"/>
+    <workbookView xWindow="28680" yWindow="-4620" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E05DA534-964F-48A7-BAA6-64E8E844F20B}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSim" sheetId="1" r:id="rId1"/>
@@ -1097,10 +1097,10 @@
         <v>6.0999999999999997E-4</v>
       </c>
       <c r="J2">
-        <v>9.7490000000000007E-3</v>
+        <v>1.04E-2</v>
       </c>
       <c r="K2">
-        <v>0.27729999999999999</v>
+        <v>0.2732</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>